<commit_message>
Separated functions for linear & log taper pots
</commit_message>
<xml_diff>
--- a/Oxygen 61 - Vb3m MIDI mapping.xlsx
+++ b/Oxygen 61 - Vb3m MIDI mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git repos\Expression-pedal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3272DB-920C-45DF-87FF-B16CF1623799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EC99F3-1588-433E-9A11-961495C1E664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1588CD5E-A643-4868-8B27-D70A09626345}"/>
+    <workbookView xWindow="30060" yWindow="0" windowWidth="26190" windowHeight="13095" xr2:uid="{1588CD5E-A643-4868-8B27-D70A09626345}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="159">
   <si>
     <t>Keyboard designator</t>
   </si>
@@ -218,18 +218,12 @@
     <t>C29</t>
   </si>
   <si>
-    <t>Replay symbol</t>
-  </si>
-  <si>
     <t>Upper right</t>
   </si>
   <si>
     <t>C30</t>
   </si>
   <si>
-    <t>Rewind symbol</t>
-  </si>
-  <si>
     <t>Other marking</t>
   </si>
   <si>
@@ -245,18 +239,6 @@
     <t>C34</t>
   </si>
   <si>
-    <t>Fast forward symbol</t>
-  </si>
-  <si>
-    <t>Stop symbol</t>
-  </si>
-  <si>
-    <t>Play symbol</t>
-  </si>
-  <si>
-    <t>Record symbol</t>
-  </si>
-  <si>
     <t>C35</t>
   </si>
   <si>
@@ -510,13 +492,34 @@
   </si>
   <si>
     <t>Program change</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>⟳  (repeat)</t>
+  </si>
+  <si>
+    <t>◀◀ (rewind)</t>
+  </si>
+  <si>
+    <t>▶▶ (ff)</t>
+  </si>
+  <si>
+    <t>■ (stop)</t>
+  </si>
+  <si>
+    <t>▶ (play)</t>
+  </si>
+  <si>
+    <t>● (record)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,6 +533,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -539,7 +549,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -547,17 +557,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -571,8 +615,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33A54D3E-A27A-47D7-A086-CFA07EA9DAC0}" name="Table1" displayName="Table1" ref="A1:G83" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33A54D3E-A27A-47D7-A086-CFA07EA9DAC0}" name="Table1" displayName="Table1" ref="A1:G83" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:G83" xr:uid="{33A54D3E-A27A-47D7-A086-CFA07EA9DAC0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G83">
+    <sortCondition ref="A1:A83"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1F02C53D-3298-4F6C-847B-1D0763576E55}" name="Keyboard designator"/>
     <tableColumn id="2" xr3:uid="{E8AF883C-28DC-4229-8044-E21D08537A3E}" name="Other marking"/>
@@ -905,267 +952,268 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2A89E8-6FF8-44FD-AD04-E980599F4A92}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="P73" sqref="P73"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
-        <v>123</v>
+      <c r="E1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="G4">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="2">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="G9">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="G11">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1174,522 +1222,522 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G12">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G14">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G15">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G16">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G18">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G19">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" t="s">
-        <v>121</v>
-      </c>
-      <c r="G23">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
+        <v>66</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G27">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G28">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G29">
-        <v>93</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33">
         <v>17</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34">
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+      <c r="E35" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G35">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G36">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G37">
         <v>31</v>
@@ -1697,10 +1745,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G38">
         <v>30</v>
@@ -1708,10 +1756,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G39">
         <v>73</v>
@@ -1719,10 +1767,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G40">
         <v>66</v>
@@ -1730,10 +1778,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G41">
         <v>70</v>
@@ -1741,10 +1789,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G42">
         <v>71</v>
@@ -1752,10 +1800,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F43" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G43">
         <v>72</v>
@@ -1763,10 +1811,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F44" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G44">
         <v>11</v>
@@ -1774,10 +1822,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F45" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G45">
         <v>21</v>
@@ -1785,10 +1833,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F46" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G46">
         <v>22</v>
@@ -1796,10 +1844,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G47">
         <v>23</v>
@@ -1807,10 +1855,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F48" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G48">
         <v>24</v>
@@ -1818,10 +1866,10 @@
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G49">
         <v>25</v>
@@ -1829,10 +1877,10 @@
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F50" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G50">
         <v>26</v>
@@ -1840,10 +1888,10 @@
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F51" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G51">
         <v>27</v>
@@ -1851,10 +1899,10 @@
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F52" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G52">
         <v>28</v>
@@ -1862,10 +1910,10 @@
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F53" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G53">
         <v>29</v>
@@ -1873,10 +1921,10 @@
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F54" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G54">
         <v>33</v>
@@ -1884,10 +1932,10 @@
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F55" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G55">
         <v>35</v>
@@ -1895,10 +1943,10 @@
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F56" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G56">
         <v>85</v>
@@ -1906,43 +1954,43 @@
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F57" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G57" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F58" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G58" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F59" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G59" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F60" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G60">
         <v>56</v>
@@ -1950,10 +1998,10 @@
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F61" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -1961,10 +2009,10 @@
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F62" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -1972,10 +2020,10 @@
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F63" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G63">
         <v>2</v>
@@ -1983,10 +2031,10 @@
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F64" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G64">
         <v>3</v>
@@ -1994,10 +2042,10 @@
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F65" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G65">
         <v>4</v>
@@ -2005,10 +2053,10 @@
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F66" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G66">
         <v>5</v>
@@ -2016,10 +2064,10 @@
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F67" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G67">
         <v>6</v>
@@ -2027,10 +2075,10 @@
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F68" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G68">
         <v>7</v>
@@ -2038,10 +2086,10 @@
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F69" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G69">
         <v>8</v>
@@ -2049,10 +2097,10 @@
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F70" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G70">
         <v>9</v>
@@ -2060,10 +2108,10 @@
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F71" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G71">
         <v>10</v>
@@ -2071,10 +2119,10 @@
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F72" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G72">
         <v>11</v>
@@ -2082,10 +2130,10 @@
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F73" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G73">
         <v>12</v>
@@ -2093,10 +2141,10 @@
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F74" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G74">
         <v>13</v>
@@ -2104,10 +2152,10 @@
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F75" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G75">
         <v>14</v>
@@ -2115,10 +2163,10 @@
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F76" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G76">
         <v>15</v>
@@ -2126,10 +2174,10 @@
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F77" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G77">
         <v>25</v>
@@ -2137,10 +2185,10 @@
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
+        <v>145</v>
+      </c>
+      <c r="F78" t="s">
         <v>151</v>
-      </c>
-      <c r="F78" t="s">
-        <v>157</v>
       </c>
       <c r="G78">
         <v>26</v>
@@ -2148,10 +2196,10 @@
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F79" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G79">
         <v>27</v>
@@ -2159,10 +2207,10 @@
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F80" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G80">
         <v>28</v>
@@ -2170,10 +2218,10 @@
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F81" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G81">
         <v>29</v>
@@ -2181,10 +2229,10 @@
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F82" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G82">
         <v>30</v>
@@ -2192,10 +2240,10 @@
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F83" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G83">
         <v>31</v>
@@ -2204,8 +2252,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>